<commit_message>
Alteração dos documentos, acréscimo do diagrama de classe
</commit_message>
<xml_diff>
--- a/Documentos/Product-backlog-Oficial.xlsx
+++ b/Documentos/Product-backlog-Oficial.xlsx
@@ -5,7 +5,7 @@
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Faculdade 2017\Sistemas 5º período\Engenharia de Software 2\Trabalhos\artefatos Oficiais\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Faculdade 2017\Repositorio\ProjetoMedicamento\Documentos\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>PRODUCT BACKLOG</t>
   </si>
@@ -45,6 +45,36 @@
   </si>
   <si>
     <t>SPRINT</t>
+  </si>
+  <si>
+    <t>chamar senhas</t>
+  </si>
+  <si>
+    <t>O sistema deve permitir a geração de senhas par o cliente</t>
+  </si>
+  <si>
+    <t>gerar senhas</t>
+  </si>
+  <si>
+    <t>O sistema deve permitir o direcionamento de cada senha aos terminais</t>
+  </si>
+  <si>
+    <t>O sistema deve manter o histórico de atendimentos</t>
+  </si>
+  <si>
+    <t>consultar atendimentos</t>
+  </si>
+  <si>
+    <t>O  sistema irá fornecer informações em tempo real de quantidade e tipos de senha</t>
+  </si>
+  <si>
+    <t>visualizar senhas</t>
+  </si>
+  <si>
+    <t>desenvolvimentos das interfaces</t>
+  </si>
+  <si>
+    <t>Desenvolvimentos das interfaces</t>
   </si>
 </sst>
 </file>
@@ -180,8 +210,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>972192</xdr:colOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>3625585</xdr:colOff>
       <xdr:row>8</xdr:row>
       <xdr:rowOff>254641</xdr:rowOff>
     </xdr:to>
@@ -543,14 +573,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BXH39"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B47" sqref="B47"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="34.75" customWidth="1"/>
-    <col min="2" max="2" width="28.375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="70.25" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="43.125" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="20.5" customWidth="1"/>
     <col min="4" max="5" width="33.375" customWidth="1"/>
     <col min="6" max="6" width="27.375" customWidth="1"/>
@@ -679,44 +709,72 @@
       <c r="G12" s="4"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="8"/>
-      <c r="B13" s="3"/>
+      <c r="A13" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>9</v>
+      </c>
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
       <c r="E13" s="3"/>
-      <c r="F13" s="3"/>
+      <c r="F13" s="3">
+        <v>1</v>
+      </c>
       <c r="G13" s="4"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="8"/>
-      <c r="B14" s="3"/>
+      <c r="A14" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>7</v>
+      </c>
       <c r="C14" s="3"/>
       <c r="D14" s="3"/>
       <c r="E14" s="3"/>
-      <c r="F14" s="3"/>
+      <c r="F14" s="3">
+        <v>2</v>
+      </c>
       <c r="G14" s="4"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="8"/>
-      <c r="B15" s="3"/>
+      <c r="A15" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>12</v>
+      </c>
       <c r="C15" s="3"/>
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
-      <c r="F15" s="3"/>
+      <c r="F15" s="3">
+        <v>3</v>
+      </c>
       <c r="G15" s="4"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="8"/>
-      <c r="B16" s="3"/>
+      <c r="A16" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>14</v>
+      </c>
       <c r="C16" s="3"/>
       <c r="D16" s="3"/>
       <c r="E16" s="3"/>
-      <c r="F16" s="3"/>
+      <c r="F16" s="3">
+        <v>4</v>
+      </c>
       <c r="G16" s="4"/>
     </row>
     <row r="17" spans="1:7 1964:1984" x14ac:dyDescent="0.25">
-      <c r="A17" s="2"/>
-      <c r="B17" s="3"/>
+      <c r="A17" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>15</v>
+      </c>
       <c r="C17" s="3"/>
       <c r="D17" s="3"/>
       <c r="E17" s="3"/>

</xml_diff>